<commit_message>
Added web socket session holder service and notifier
</commit_message>
<xml_diff>
--- a/documents/Models.ods.xlsx
+++ b/documents/Models.ods.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1261,6 +1262,1944 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Прямоугольник 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762251" y="1819275"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Public</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Controller</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Прямоугольник 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762251" y="2562225"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Private</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Controller</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Прямоугольник 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2743201" y="3257550"/>
+          <a:ext cx="1371600" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS handler</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Прямоугольник 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7562850" y="1819275"/>
+          <a:ext cx="2019300" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Allow registration filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Прямоугольник 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7572375" y="2543175"/>
+          <a:ext cx="2019300" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Deny registration filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Прямоугольник 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4819651" y="3248025"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS session filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Прямая со стрелкой 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4114801" y="3424238"/>
+          <a:ext cx="704850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Соединительная линия уступом 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5936458" y="1612108"/>
+          <a:ext cx="1185860" cy="2085974"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Прямая со стрелкой 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095751" y="1995488"/>
+          <a:ext cx="3467099" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Прямая со стрелкой 19"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4095751" y="2719388"/>
+          <a:ext cx="3476624" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Прямоугольник 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10306051" y="2171700"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Type</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> request router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Прямоугольник 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363451" y="1628775"/>
+          <a:ext cx="2009774" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Authorization router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Прямоугольник 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12372975" y="2162175"/>
+          <a:ext cx="2019299" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Messenger</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Прямоугольник 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363450" y="2695575"/>
+          <a:ext cx="2038349" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Profile</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Прямая со стрелкой 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9582150" y="1995488"/>
+          <a:ext cx="723901" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Прямая со стрелкой 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9591675" y="2347913"/>
+          <a:ext cx="714376" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Прямая со стрелкой 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="24" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11639551" y="1804988"/>
+          <a:ext cx="723900" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Прямая со стрелкой 36"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="25" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11639551" y="2338388"/>
+          <a:ext cx="733424" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Прямая со стрелкой 38"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="26" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11639551" y="2347913"/>
+          <a:ext cx="723899" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Прямоугольник 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15049500" y="1743075"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Прямоугольник 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="2552700"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>JWT filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Прямая со стрелкой 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="41" idx="3"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2038350" y="2728913"/>
+          <a:ext cx="723901" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Прямоугольник 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="4000500"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS session holder</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Прямая со стрелкой 45"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="44" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3419475" y="3609975"/>
+          <a:ext cx="9526" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Прямая со стрелкой 47"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="0"/>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3419475" y="3609975"/>
+          <a:ext cx="9526" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Соединительная линия уступом 51"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="23" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6153151" y="2524125"/>
+          <a:ext cx="4819650" cy="900113"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Прямоугольник 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15201900" y="1895475"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Прямоугольник 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15354300" y="2047875"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Прямоугольник 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15506700" y="2200275"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Прямоугольник 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15659100" y="2352675"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Прямоугольник 62"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15811500" y="2505075"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Прямоугольник 63"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15963900" y="2657475"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Прямоугольник 64"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486399" y="3981450"/>
+          <a:ext cx="2047876" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS multicast</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> notifier</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Прямая со стрелкой 66"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="65" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4086225" y="4157663"/>
+          <a:ext cx="1400174" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Соединительная линия уступом 68"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="64" idx="2"/>
+          <a:endCxn id="65" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11508582" y="-983456"/>
+          <a:ext cx="1166813" cy="9115425"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -1550,7 +3489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
@@ -29427,4 +31366,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Web socket notifier (#44)
* Added web socket session holder service and notifier

* Sonar lint fixes
</commit_message>
<xml_diff>
--- a/documents/Models.ods.xlsx
+++ b/documents/Models.ods.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1261,6 +1262,1944 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Прямоугольник 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762251" y="1819275"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Public</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Controller</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Прямоугольник 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762251" y="2562225"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Private</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Controller</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Прямоугольник 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2743201" y="3257550"/>
+          <a:ext cx="1371600" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS handler</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Прямоугольник 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7562850" y="1819275"/>
+          <a:ext cx="2019300" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Allow registration filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Прямоугольник 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7572375" y="2543175"/>
+          <a:ext cx="2019300" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Deny registration filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Прямоугольник 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4819651" y="3248025"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS session filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Прямая со стрелкой 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4114801" y="3424238"/>
+          <a:ext cx="704850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Соединительная линия уступом 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5936458" y="1612108"/>
+          <a:ext cx="1185860" cy="2085974"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Прямая со стрелкой 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095751" y="1995488"/>
+          <a:ext cx="3467099" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Прямая со стрелкой 19"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4095751" y="2719388"/>
+          <a:ext cx="3476624" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Прямоугольник 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10306051" y="2171700"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Type</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> request router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Прямоугольник 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363451" y="1628775"/>
+          <a:ext cx="2009774" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Authorization router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Прямоугольник 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12372975" y="2162175"/>
+          <a:ext cx="2019299" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Messenger</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Прямоугольник 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363450" y="2695575"/>
+          <a:ext cx="2038349" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Profile</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> router</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Прямая со стрелкой 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9582150" y="1995488"/>
+          <a:ext cx="723901" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Прямая со стрелкой 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9591675" y="2347913"/>
+          <a:ext cx="714376" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Прямая со стрелкой 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="24" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11639551" y="1804988"/>
+          <a:ext cx="723900" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Прямая со стрелкой 36"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="25" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11639551" y="2338388"/>
+          <a:ext cx="733424" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Прямая со стрелкой 38"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="26" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11639551" y="2347913"/>
+          <a:ext cx="723899" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Прямоугольник 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15049500" y="1743075"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Прямоугольник 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="2552700"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>JWT filter</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Прямая со стрелкой 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="41" idx="3"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2038350" y="2728913"/>
+          <a:ext cx="723901" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Прямоугольник 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="4000500"/>
+          <a:ext cx="1333500" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS session holder</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Прямая со стрелкой 45"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="44" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3419475" y="3609975"/>
+          <a:ext cx="9526" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Прямая со стрелкой 47"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="0"/>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3419475" y="3609975"/>
+          <a:ext cx="9526" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Соединительная линия уступом 51"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="23" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6153151" y="2524125"/>
+          <a:ext cx="4819650" cy="900113"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Прямоугольник 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15201900" y="1895475"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Прямоугольник 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15354300" y="2047875"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Прямоугольник 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15506700" y="2200275"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Прямоугольник 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15659100" y="2352675"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Прямоугольник 62"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15811500" y="2505075"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Прямоугольник 63"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15963900" y="2657475"/>
+          <a:ext cx="1371600" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Handlers</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Прямоугольник 64"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486399" y="3981450"/>
+          <a:ext cx="2047876" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>WS multicast</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> notifier</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Прямая со стрелкой 66"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="65" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4086225" y="4157663"/>
+          <a:ext cx="1400174" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Соединительная линия уступом 68"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="64" idx="2"/>
+          <a:endCxn id="65" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11508582" y="-983456"/>
+          <a:ext cx="1166813" cy="9115425"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -1550,7 +3489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
@@ -29427,4 +31366,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added contacts addition and deletion.
</commit_message>
<xml_diff>
--- a/documents/Models.ods.xlsx
+++ b/documents/Models.ods.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="130">
   <si>
     <t>Conversation</t>
   </si>
@@ -400,6 +400,12 @@
   <si>
     <t>смещение</t>
   </si>
+  <si>
+    <t>table contact_phone_numbers</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
 </sst>
 </file>
 
@@ -502,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -547,11 +553,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -591,6 +612,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -627,7 +649,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16354425" y="1495425"/>
+          <a:off x="16411575" y="1495425"/>
           <a:ext cx="352425" cy="581025"/>
           <a:chOff x="3219450" y="4057725"/>
           <a:chExt cx="314400" cy="104700"/>
@@ -683,7 +705,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16354425" y="3276600"/>
+          <a:off x="16411575" y="3276600"/>
           <a:ext cx="409575" cy="552450"/>
           <a:chOff x="4476750" y="1857375"/>
           <a:chExt cx="1333500" cy="1333500"/>
@@ -1258,6 +1280,50 @@
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Прямая соединительная линия 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13477875" y="428625"/>
+          <a:ext cx="1504950" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -3489,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="15" customHeight="1"/>
@@ -3501,7 +3567,8 @@
     <col min="4" max="4" width="19.625" customWidth="1"/>
     <col min="5" max="5" width="85.5" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="8" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="10.625" customWidth="1"/>
     <col min="9" max="9" width="18.375" customWidth="1"/>
     <col min="10" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="29.375" customWidth="1"/>
@@ -3521,6 +3588,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="22" t="s">
+        <v>128</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -3546,7 +3616,9 @@
       <c r="D2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="I2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="3" t="s">
         <v>1</v>
@@ -3579,7 +3651,9 @@
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="I3" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -3614,6 +3688,9 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="I4" s="39" t="s">
+        <v>17</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -3711,7 +3788,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="F7" s="10" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3738,9 +3815,6 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="F8" s="10" t="s">
-        <v>5</v>
-      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">

</xml_diff>

<commit_message>
Added contacts addition and deletion. (#45)
</commit_message>
<xml_diff>
--- a/documents/Models.ods.xlsx
+++ b/documents/Models.ods.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="130">
   <si>
     <t>Conversation</t>
   </si>
@@ -400,6 +400,12 @@
   <si>
     <t>смещение</t>
   </si>
+  <si>
+    <t>table contact_phone_numbers</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
 </sst>
 </file>
 
@@ -502,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -547,11 +553,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -591,6 +612,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -627,7 +649,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16354425" y="1495425"/>
+          <a:off x="16411575" y="1495425"/>
           <a:ext cx="352425" cy="581025"/>
           <a:chOff x="3219450" y="4057725"/>
           <a:chExt cx="314400" cy="104700"/>
@@ -683,7 +705,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16354425" y="3276600"/>
+          <a:off x="16411575" y="3276600"/>
           <a:ext cx="409575" cy="552450"/>
           <a:chOff x="4476750" y="1857375"/>
           <a:chExt cx="1333500" cy="1333500"/>
@@ -1258,6 +1280,50 @@
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Прямая соединительная линия 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13477875" y="428625"/>
+          <a:ext cx="1504950" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -3489,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="15" customHeight="1"/>
@@ -3501,7 +3567,8 @@
     <col min="4" max="4" width="19.625" customWidth="1"/>
     <col min="5" max="5" width="85.5" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="8" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="10.625" customWidth="1"/>
     <col min="9" max="9" width="18.375" customWidth="1"/>
     <col min="10" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="29.375" customWidth="1"/>
@@ -3521,6 +3588,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="22" t="s">
+        <v>128</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -3546,7 +3616,9 @@
       <c r="D2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="I2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="3" t="s">
         <v>1</v>
@@ -3579,7 +3651,9 @@
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="I3" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -3614,6 +3688,9 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="I4" s="39" t="s">
+        <v>17</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -3711,7 +3788,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="F7" s="10" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3738,9 +3815,6 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="F8" s="10" t="s">
-        <v>5</v>
-      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">

</xml_diff>